<commit_message>
Added northeast, northwest and south dummies
</commit_message>
<xml_diff>
--- a/documentazione_storico_versione11.1.xlsx
+++ b/documentazione_storico_versione11.1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{D5E025A3-0631-4FB0-B252-4F62B7C83719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ED97DDD-53A3-4355-978E-2F98DEC60EBA}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{D5E025A3-0631-4FB0-B252-4F62B7C83719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F76EA2F4-D1E7-4169-8D65-B81BE63D5B31}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" tabRatio="920" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28689,9 +28689,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31323,7 +31323,7 @@
       <c r="X67" s="5"/>
       <c r="Y67"/>
     </row>
-    <row r="68" spans="1:25" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68" t="s">
         <v>91</v>
@@ -31362,7 +31362,7 @@
       <c r="X68" s="5"/>
       <c r="Y68"/>
     </row>
-    <row r="69" spans="1:25" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69" s="28" t="s">
         <v>92</v>
@@ -31973,7 +31973,7 @@
       <c r="X84" s="5"/>
       <c r="Y84"/>
     </row>
-    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85" s="28" t="s">
         <v>108</v>
@@ -32476,7 +32476,7 @@
       <c r="X97" s="5"/>
       <c r="Y97"/>
     </row>
-    <row r="98" spans="1:25" ht="72" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:25" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98" s="28" t="s">
         <v>121</v>
@@ -32499,7 +32499,7 @@
       </c>
       <c r="Y98"/>
     </row>
-    <row r="99" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99" s="28" t="s">
         <v>122</v>
@@ -32522,7 +32522,7 @@
       </c>
       <c r="Y99"/>
     </row>
-    <row r="100" spans="1:25" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100" s="28" t="s">
         <v>507</v>
@@ -32545,7 +32545,7 @@
       </c>
       <c r="Y100"/>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101" s="28" t="s">
         <v>123</v>
@@ -38719,7 +38719,7 @@
       <c r="X329" s="59"/>
       <c r="Y329" s="52"/>
     </row>
-    <row r="330" spans="1:25" s="56" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:25" s="56" customFormat="1" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="52"/>
       <c r="B330" s="56" t="s">
         <v>1054</v>
@@ -38801,11 +38801,9 @@
   <autoFilter ref="A1:X331" xr:uid="{00000000-0009-0000-0000-000003000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="QUALP10"/>
-        <filter val="QUALP10N"/>
-        <filter val="QUALP3"/>
-        <filter val="QUALP7"/>
-        <filter val="QUALP7N"/>
+        <filter val="AREA3"/>
+        <filter val="AREA5"/>
+        <filter val="NASCAREA"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -44545,12 +44543,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009751835CD414CC46B42FC830D124F282" ma:contentTypeVersion="3" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="734608599edb9e534b5c1f5aed05870b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0ca655e-bd60-4883-8c29-d6111a25fe13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b929488029f66b1850ce1557473a41e" ns2:_="">
     <xsd:import namespace="f0ca655e-bd60-4883-8c29-d6111a25fe13"/>
@@ -44698,6 +44690,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -44708,22 +44706,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B51DDAD-6AFF-4837-8984-9F439B39B231}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f0ca655e-bd60-4883-8c29-d6111a25fe13"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B43AA01A-6291-4146-A29D-1ECC48A0ABAE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44741,6 +44723,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B51DDAD-6AFF-4837-8984-9F439B39B231}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f0ca655e-bd60-4883-8c29-d6111a25fe13"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59EB524F-E0B3-40C0-AF3E-75CDFAF009E6}">
   <ds:schemaRefs>

</xml_diff>